<commit_message>
Adding new dals, chaas and rice recipe
</commit_message>
<xml_diff>
--- a/Drinks/Pudina chaas.xlsx
+++ b/Drinks/Pudina chaas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nandi\Google Drive\recipies\Drinks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127B4FD8-2E24-4777-97AC-62BE3C5F1D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5124F0D4-E39C-4EAD-A293-32698852EDB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CBC1288-2A94-44F0-92DE-D9C7067027C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>How many servings</t>
   </si>
@@ -121,12 +121,6 @@
   </si>
   <si>
     <t>water/curd ratio</t>
-  </si>
-  <si>
-    <t>water in first go</t>
-  </si>
-  <si>
-    <t>water in second go</t>
   </si>
   <si>
     <t>Base Recipe</t>
@@ -739,7 +733,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +753,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -768,13 +762,13 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -783,14 +777,14 @@
       </c>
       <c r="B2" s="7">
         <f>E2*F2/G2</f>
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2">
         <v>2.5</v>
@@ -811,15 +805,15 @@
         <v>23</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B13" si="0">E2*F3/G3</f>
-        <v>11</v>
+        <f t="shared" ref="B3:B8" si="0">E2*F3/G3</f>
+        <v>8.25</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
         <v>5.5</v>
@@ -834,14 +828,14 @@
       </c>
       <c r="B4" s="7">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2">
         <v>0.6</v>
@@ -856,14 +850,14 @@
       </c>
       <c r="B5" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
@@ -878,14 +872,14 @@
       </c>
       <c r="B6" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -900,14 +894,14 @@
       </c>
       <c r="B7" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2">
         <v>1.5</v>
@@ -922,17 +916,17 @@
       </c>
       <c r="B8" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="2">
         <v>2</v>
@@ -948,13 +942,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="2">
-        <f>7.75-B2</f>
-        <v>2.75</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="2"/>
@@ -962,13 +951,8 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="7">
-        <f>B3-B10</f>
-        <v>8.25</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>

</xml_diff>